<commit_message>
made gui optional, added troop support
</commit_message>
<xml_diff>
--- a/topBot.xlsx
+++ b/topBot.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
   <si>
     <t>Alaska</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Central America</t>
+  </si>
+  <si>
+    <t>bonus</t>
+  </si>
+  <si>
+    <t>Africa</t>
   </si>
 </sst>
 </file>
@@ -744,7 +750,595 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="86">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1056,11 +1650,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS43"/>
+  <dimension ref="A1:AT43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AT43" sqref="AT43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1665,7 @@
     <col min="45" max="45" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1204,8 +1798,11 @@
       <c r="AS1" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="AT1" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1341,8 +1938,11 @@
       <c r="AS2" t="s">
         <v>56</v>
       </c>
+      <c r="AT2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1478,8 +2078,11 @@
       <c r="AS3" t="s">
         <v>56</v>
       </c>
+      <c r="AT3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1615,8 +2218,11 @@
       <c r="AS4" t="s">
         <v>56</v>
       </c>
+      <c r="AT4">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1752,8 +2358,11 @@
       <c r="AS5" t="s">
         <v>56</v>
       </c>
+      <c r="AT5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1889,8 +2498,11 @@
       <c r="AS6" t="s">
         <v>56</v>
       </c>
+      <c r="AT6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2026,8 +2638,11 @@
       <c r="AS7" t="s">
         <v>56</v>
       </c>
+      <c r="AT7">
+        <v>5</v>
+      </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2163,8 +2778,11 @@
       <c r="AS8" t="s">
         <v>56</v>
       </c>
+      <c r="AT8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2300,8 +2918,11 @@
       <c r="AS9" t="s">
         <v>56</v>
       </c>
+      <c r="AT9">
+        <v>5</v>
+      </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2437,8 +3058,11 @@
       <c r="AS10" t="s">
         <v>56</v>
       </c>
+      <c r="AT10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2574,8 +3198,11 @@
       <c r="AS11" t="s">
         <v>57</v>
       </c>
+      <c r="AT11">
+        <v>2</v>
+      </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2711,8 +3338,11 @@
       <c r="AS12" t="s">
         <v>57</v>
       </c>
+      <c r="AT12">
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2848,8 +3478,11 @@
       <c r="AS13" t="s">
         <v>57</v>
       </c>
+      <c r="AT13">
+        <v>2</v>
+      </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2985,8 +3618,11 @@
       <c r="AS14" t="s">
         <v>57</v>
       </c>
+      <c r="AT14">
+        <v>2</v>
+      </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -3122,8 +3758,11 @@
       <c r="AS15" t="s">
         <v>58</v>
       </c>
+      <c r="AT15">
+        <v>5</v>
+      </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3259,8 +3898,11 @@
       <c r="AS16" t="s">
         <v>58</v>
       </c>
+      <c r="AT16">
+        <v>5</v>
+      </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -3396,8 +4038,11 @@
       <c r="AS17" t="s">
         <v>58</v>
       </c>
+      <c r="AT17">
+        <v>5</v>
+      </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3533,8 +4178,11 @@
       <c r="AS18" t="s">
         <v>58</v>
       </c>
+      <c r="AT18">
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -3670,8 +4318,11 @@
       <c r="AS19" t="s">
         <v>58</v>
       </c>
+      <c r="AT19">
+        <v>5</v>
+      </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3807,8 +4458,11 @@
       <c r="AS20" t="s">
         <v>58</v>
       </c>
+      <c r="AT20">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -3944,8 +4598,11 @@
       <c r="AS21" t="s">
         <v>58</v>
       </c>
+      <c r="AT21">
+        <v>5</v>
+      </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -4079,10 +4736,13 @@
         <v>3</v>
       </c>
       <c r="AS22" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="AT22">
+        <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>48</v>
       </c>
@@ -4216,10 +4876,13 @@
         <v>3</v>
       </c>
       <c r="AS23" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="AT23">
+        <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -4353,10 +5016,13 @@
         <v>3</v>
       </c>
       <c r="AS24" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="AT24">
+        <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -4490,10 +5156,13 @@
         <v>3</v>
       </c>
       <c r="AS25" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="AT25">
+        <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -4627,10 +5296,13 @@
         <v>3</v>
       </c>
       <c r="AS26" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="AT26">
+        <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -4764,10 +5436,13 @@
         <v>3</v>
       </c>
       <c r="AS27" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="AT27">
+        <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -4903,8 +5578,11 @@
       <c r="AS28" t="s">
         <v>59</v>
       </c>
+      <c r="AT28">
+        <v>7</v>
+      </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -5040,8 +5718,11 @@
       <c r="AS29" t="s">
         <v>59</v>
       </c>
+      <c r="AT29">
+        <v>7</v>
+      </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -5177,8 +5858,11 @@
       <c r="AS30" t="s">
         <v>59</v>
       </c>
+      <c r="AT30">
+        <v>7</v>
+      </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -5314,8 +5998,11 @@
       <c r="AS31" t="s">
         <v>59</v>
       </c>
+      <c r="AT31">
+        <v>7</v>
+      </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -5451,8 +6138,11 @@
       <c r="AS32" t="s">
         <v>59</v>
       </c>
+      <c r="AT32">
+        <v>7</v>
+      </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -5588,8 +6278,11 @@
       <c r="AS33" t="s">
         <v>59</v>
       </c>
+      <c r="AT33">
+        <v>7</v>
+      </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -5725,8 +6418,11 @@
       <c r="AS34" t="s">
         <v>59</v>
       </c>
+      <c r="AT34">
+        <v>7</v>
+      </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -5862,8 +6558,11 @@
       <c r="AS35" t="s">
         <v>59</v>
       </c>
+      <c r="AT35">
+        <v>7</v>
+      </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -5999,8 +6698,11 @@
       <c r="AS36" t="s">
         <v>59</v>
       </c>
+      <c r="AT36">
+        <v>7</v>
+      </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -6136,8 +6838,11 @@
       <c r="AS37" t="s">
         <v>59</v>
       </c>
+      <c r="AT37">
+        <v>7</v>
+      </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -6273,8 +6978,11 @@
       <c r="AS38" t="s">
         <v>59</v>
       </c>
+      <c r="AT38">
+        <v>7</v>
+      </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -6410,8 +7118,11 @@
       <c r="AS39" t="s">
         <v>59</v>
       </c>
+      <c r="AT39">
+        <v>7</v>
+      </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
@@ -6547,8 +7258,11 @@
       <c r="AS40" t="s">
         <v>60</v>
       </c>
+      <c r="AT40">
+        <v>2</v>
+      </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -6684,8 +7398,11 @@
       <c r="AS41" t="s">
         <v>60</v>
       </c>
+      <c r="AT41">
+        <v>2</v>
+      </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
@@ -6821,8 +7538,11 @@
       <c r="AS42" t="s">
         <v>60</v>
       </c>
+      <c r="AT42">
+        <v>2</v>
+      </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
@@ -6958,9 +7678,12 @@
       <c r="AS43" t="s">
         <v>60</v>
       </c>
+      <c r="AT43">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:AR43">
+  <conditionalFormatting sqref="B2:AR43 AT2:AT43">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="-1"/>
@@ -6971,10 +7694,10 @@
         <color rgb="FF0070C0"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="1" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>